<commit_message>
improved translation in IT template
</commit_message>
<xml_diff>
--- a/bulk-upload-templates/it/IT_E-Label_Template.xlsx
+++ b/bulk-upload-templates/it/IT_E-Label_Template.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gigi/Desktop/Imero/e-label.io/bulk-upload-templates/it/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxbauer/workspace/vs_code/misc/e-label.io/bulk-upload-templates/it/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27AADED-F6B5-824B-8C50-19A3269442EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343BBCA3-24A7-864A-9DFC-AD245FFE984B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1160" windowWidth="30240" windowHeight="15580" xr2:uid="{42B7CF4C-2976-4744-81A6-4766AD4B0A9A}"/>
   </bookViews>
   <sheets>
     <sheet name="E-Label Upload" sheetId="1" r:id="rId1"/>
-    <sheet name="Erlaubte Zutaten" sheetId="2" r:id="rId2"/>
+    <sheet name="Erlaubte Zutaten" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>Ingredienti 6</t>
-  </si>
-  <si>
-    <t>Uva</t>
   </si>
   <si>
     <t>Saccarosio</t>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>Monaco</t>
+  </si>
+  <si>
+    <t>Uve</t>
   </si>
 </sst>
 </file>
@@ -462,7 +462,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -483,9 +483,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -523,7 +523,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -629,7 +629,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -771,7 +771,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -783,7 +783,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1:J1048576"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -858,7 +858,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="31">
         <v>2023</v>
@@ -867,7 +867,7 @@
         <v>750</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G2" s="32">
         <v>12.3</v>
@@ -879,10 +879,10 @@
         <v>11</v>
       </c>
       <c r="J2" s="33" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="K2" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L2" s="33"/>
       <c r="M2" s="33"/>
@@ -18856,7 +18856,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18875,147 +18875,147 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="35"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="35"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="37" t="s">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="37" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
+      <c r="K4" s="36"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="36"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="37" t="s">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="37" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="37" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="37" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="37" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="37" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="37" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="37" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="37" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="37" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="37" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="37" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="37" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="37" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="37" t="s">
+      <c r="K12" s="36"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="K12" s="36"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="37" t="s">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="37" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="37" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="37" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="37" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="37" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="37" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="K18" s="36"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="37" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="37" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="K18" s="36"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="37" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="37" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="37" t="s">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="37" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="37" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="37" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="37" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="37" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="37" t="s">
+      <c r="K23" s="36"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="K23" s="36"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="37" t="s">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="37" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="37" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="37" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="37" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="37" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="37" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="37" t="s">
-        <v>41</v>
-      </c>
-    </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>